<commit_message>
update database field types
</commit_message>
<xml_diff>
--- a/database_design/magento24_notes.xlsx
+++ b/database_design/magento24_notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HTran14\Desktop\design\database_design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7988781C-AC91-4EF3-8CA4-DF5CA470F3FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE326908-93A2-4EA9-9FCB-2256844C789C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,6 +18,7 @@
     <sheet name="Tables" sheetId="3" r:id="rId3"/>
     <sheet name="prod_detail_page" sheetId="4" r:id="rId4"/>
     <sheet name="ecommerce" sheetId="7" r:id="rId5"/>
+    <sheet name="Sheet3" sheetId="8" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$E$882</definedName>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3010" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3067" uniqueCount="230">
   <si>
     <t>function</t>
   </si>
@@ -742,9 +743,6 @@
     <t>enum of string</t>
   </si>
   <si>
-    <t>select, input, textarea, multiselect, boolean</t>
-  </si>
-  <si>
     <t>decimal(20,6)</t>
   </si>
   <si>
@@ -773,6 +771,9 @@
   </si>
   <si>
     <t>int, decimal, varchar, text, datetime</t>
+  </si>
+  <si>
+    <t>input, multiinput, select, multiselect, boolean, password</t>
   </si>
 </sst>
 </file>
@@ -803,12 +804,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -823,7 +830,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -839,6 +846,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11685,8 +11693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58AD0879-7070-416A-8C3F-2949C772A589}">
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11774,15 +11782,15 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -11790,7 +11798,7 @@
         <v>182</v>
       </c>
       <c r="B12" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -11849,12 +11857,12 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -11935,10 +11943,10 @@
         <v>200</v>
       </c>
       <c r="D28" t="s">
-        <v>219</v>
+        <v>229</v>
       </c>
       <c r="E28" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -11951,18 +11959,18 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D30" t="s">
+        <v>226</v>
+      </c>
+      <c r="E30" t="s">
         <v>227</v>
-      </c>
-      <c r="E30" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -12035,12 +12043,12 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -12116,12 +12124,12 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -12168,7 +12176,7 @@
         <v>203</v>
       </c>
       <c r="D59" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -12197,12 +12205,12 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -12249,7 +12257,7 @@
         <v>203</v>
       </c>
       <c r="D70" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -12278,12 +12286,12 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -12330,7 +12338,7 @@
         <v>203</v>
       </c>
       <c r="D81" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -12359,12 +12367,12 @@
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -12440,12 +12448,237 @@
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>225</v>
+        <v>224</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{791567FA-DC79-4F29-B499-EB58D44E0434}">
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="6" width="12.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B4" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>184</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>182</v>
+      </c>
+      <c r="B10" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>184</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>182</v>
+      </c>
+      <c r="B13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>184</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>182</v>
+      </c>
+      <c r="B16" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>184</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>182</v>
+      </c>
+      <c r="B19" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>184</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>182</v>
+      </c>
+      <c r="B22" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>184</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>182</v>
+      </c>
+      <c r="B25" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>184</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>215</v>
       </c>
     </row>
   </sheetData>

</xml_diff>